<commit_message>
Arrumando grafico number_of_laps x average_lap_time
</commit_message>
<xml_diff>
--- a/Models/classificacao.xlsx
+++ b/Models/classificacao.xlsx
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marcelo Mastroianni</t>
+          <t>Virtualdo Pereira</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Italiano</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -491,14 +491,14 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:01:25.120547</t>
+          <t>0:01:07.600338</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Max Overseas</t>
+          <t>George Nicholson</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -508,41 +508,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Scuderia Archi Del'lappa</t>
+          <t>Empire GP</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0:01:27.135867</t>
+          <t>0:01:07.888590</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Öster Tasion</t>
+          <t>Giorgio Bussagna</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dani Ela Racing</t>
+          <t>Empire GP</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -551,28 +551,28 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:01:28.317524</t>
+          <t>0:01:07.976509</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Chu Pak-UI</t>
+          <t>Umineko Portela</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>North-Korea</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Missuga Motors</t>
+          <t>CoperSucca</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -581,28 +581,28 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:01:28.448320</t>
+          <t>0:01:08.038231</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Giorgio Bussagna</t>
+          <t>Abílio de Souza</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Equatorial Guinea</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Empire GP</t>
+          <t>Gurgel RP</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -611,28 +611,28 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:01:28.765903</t>
+          <t>0:01:08.223204</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>George Nicholson</t>
+          <t>Leonardo Henrique</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Empire GP</t>
+          <t>CoperSucca</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:01:29.284235</t>
+          <t>0:01:08.254064</t>
         </is>
       </c>
     </row>
@@ -671,139 +671,139 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:01:29.424128</t>
+          <t>0:01:08.287349</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chavez Tigrón</t>
+          <t>Chu Pak-UI</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>North-Korea</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Scuderia Archi Del'lappa</t>
+          <t>Missuga Motors</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:01:30.054239</t>
+          <t>0:01:08.383341</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Kahn Templani Efdoux</t>
+          <t>Öster Tasion</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Aoi Yu Racers</t>
+          <t>Dani Ela Racing</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:01:30.802210</t>
+          <t>0:01:08.503860</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Acistino Effoum</t>
+          <t>Jorge Pelado</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Equatorial Guinea</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Aoi Yu Racers</t>
+          <t>Missuga Motors</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:01:30.849184</t>
+          <t>0:01:08.520360</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Umineko Portela</t>
+          <t>Max Overseas</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CoperSucca</t>
+          <t>Scuderia Archi Del'lappa</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:01:31.487794</t>
+          <t>0:01:08.523868</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Abílio de Souza</t>
+          <t>Thravekis Galludis</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -821,28 +821,28 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:01:32.269797</t>
+          <t>0:01:08.562919</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Thravekis Galludis</t>
+          <t>Marcelo Mastroianni</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Italiano</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Gurgel RP</t>
+          <t>ACS Racing</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -851,97 +851,97 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:01:32.801973</t>
+          <t>0:01:08.827894</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Leonardo Henrique</t>
+          <t>Chavez Tigrón</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CoperSucca</t>
+          <t>Scuderia Archi Del'lappa</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:01:33.530324</t>
+          <t>0:01:08.914482</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Virtualdo Pereira</t>
+          <t>Kahn Templani Efdoux</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>ACS Racing</t>
+          <t>Aoi Yu Racers</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:01:34.630189</t>
+          <t>0:01:09.006399</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Jorge Pelado</t>
+          <t>Acistino Effoum</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Missuga Motors</t>
+          <t>Aoi Yu Racers</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Hard</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:01:35.288965</t>
+          <t>0:01:09.258644</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Arrumando IA do pitstop
</commit_message>
<xml_diff>
--- a/Models/classificacao.xlsx
+++ b/Models/classificacao.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,37 +468,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Virtualdo Pereira</t>
+          <t>Esteban Ocon</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ACS Racing</t>
+          <t>Renault</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:01:07.600338</t>
+          <t>0:01:20.271098</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>George Nicholson</t>
+          <t>Lando Norris</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Empire GP</t>
+          <t>McLaren</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,432 +516,552 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0:01:07.888590</t>
+          <t>0:01:20.625276</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Giorgio Bussagna</t>
+          <t>Mick Schumacher</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Empire GP</t>
+          <t>Haas</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:01:07.976509</t>
+          <t>0:01:20.642260</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Umineko Portela</t>
+          <t>Carlos Sainz Jr</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CoperSucca</t>
+          <t>Ferrari</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:01:08.038231</t>
+          <t>0:01:20.657936</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Abílio de Souza</t>
+          <t>Lewis Hamilton</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gurgel RP</t>
+          <t>Mercedes</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:01:08.223204</t>
+          <t>0:01:20.744348</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Leonardo Henrique</t>
+          <t>Valteri Bottas</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CoperSucca</t>
+          <t>Mercedes</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:01:08.254064</t>
+          <t>0:01:20.769499</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Chic Kane</t>
+          <t>Fernando Alonso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Dani Ela Racing</t>
+          <t>Renault</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:01:08.287349</t>
+          <t>0:01:20.791443</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chu Pak-UI</t>
+          <t>Sebastian Vettel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>North-Korea</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Missuga Motors</t>
+          <t>Aston Martin</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:01:08.383341</t>
+          <t>0:01:20.935625</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Öster Tasion</t>
+          <t>Charles Lecerc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Monaco</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dani Ela Racing</t>
+          <t>Ferrari</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:01:08.503860</t>
+          <t>0:01:20.942232</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jorge Pelado</t>
+          <t>Daniel Ricciardo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Equatorial Guinea</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Missuga Motors</t>
+          <t>McLaren</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:01:08.520360</t>
+          <t>0:01:21.024493</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Max Overseas</t>
+          <t>Nikita Mazepin</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Scuderia Archi Del'lappa</t>
+          <t>Haas</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:01:08.523868</t>
+          <t>0:01:21.147089</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Thravekis Galludis</t>
+          <t>Pierre Gasly</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gurgel RP</t>
+          <t>Alpha Tauri</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:01:08.562919</t>
+          <t>0:01:21.238110</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Marcelo Mastroianni</t>
+          <t>Sergio Pérez</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Italiano</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ACS Racing</t>
+          <t>Red Bull</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Medium</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:01:08.827894</t>
+          <t>0:01:21.392578</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chavez Tigrón</t>
+          <t>Lance Stroll</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Scuderia Archi Del'lappa</t>
+          <t>Aston Martin</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:01:08.914482</t>
+          <t>0:01:21.507750</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kahn Templani Efdoux</t>
+          <t>George Russel</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Aoi Yu Racers</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:01:09.006399</t>
+          <t>0:01:21.580007</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Acistino Effoum</t>
+          <t>Kimi Raikkonen</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Aoi Yu Racers</t>
+          <t>Alfa-Romeo</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Hard</t>
+          <t>Soft</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:01:09.258644</t>
+          <t>0:01:21.585747</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Yuki Tsunoda</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alpha Tauri</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>22</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Soft</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0:01:21.685020</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Nicholas Latifi</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Williams</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Soft</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>0:01:21.782664</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Max Verstappen</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Red Bull</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>33</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Soft</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>0:01:21.842005</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Antonio Giovinazzi</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alfa-Romeo</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>99</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Soft</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>0:01:21.861092</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Pitstop nas ultimas 15% das voltas proibido e arrumando gap_to_leader
</commit_message>
<xml_diff>
--- a/Models/classificacao.xlsx
+++ b/Models/classificacao.xlsx
@@ -468,12 +468,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Esteban Ocon</t>
+          <t>Fernando Alonso</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -491,14 +491,14 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0:01:20.271098</t>
+          <t>0:01:28.926388</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lando Norris</t>
+          <t>Lewis Hamilton</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -508,11 +508,11 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>McLaren</t>
+          <t>Mercedes</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -521,28 +521,28 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0:01:20.625276</t>
+          <t>0:01:28.997629</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mick Schumacher</t>
+          <t>Carlos Sainz Jr</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Haas</t>
+          <t>Ferrari</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -551,28 +551,28 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0:01:20.642260</t>
+          <t>0:01:29.044263</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Carlos Sainz Jr</t>
+          <t>Max Verstappen</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ferrari</t>
+          <t>Red Bull</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -581,28 +581,28 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0:01:20.657936</t>
+          <t>0:01:29.047641</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lewis Hamilton</t>
+          <t>Mick Schumacher</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mercedes</t>
+          <t>Haas</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -611,28 +611,28 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0:01:20.744348</t>
+          <t>0:01:29.191375</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Valteri Bottas</t>
+          <t>Esteban Ocon</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mercedes</t>
+          <t>Renault</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -641,28 +641,28 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0:01:20.769499</t>
+          <t>0:01:29.222135</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Fernando Alonso</t>
+          <t>Daniel Ricciardo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Renault</t>
+          <t>McLaren</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -671,28 +671,28 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0:01:20.791443</t>
+          <t>0:01:29.361194</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sebastian Vettel</t>
+          <t>Charles Leclerc</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Monaco</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Aston Martin</t>
+          <t>Ferrari</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -701,28 +701,28 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0:01:20.935625</t>
+          <t>0:01:29.368085</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Charles Lecerc</t>
+          <t>Lando Norris</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Monaco</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ferrari</t>
+          <t>McLaren</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -731,28 +731,28 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0:01:20.942232</t>
+          <t>0:01:29.373747</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Daniel Ricciardo</t>
+          <t>Valteri Bottas</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>McLaren</t>
+          <t>Mercedes</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -761,28 +761,28 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0:01:21.024493</t>
+          <t>0:01:29.439958</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nikita Mazepin</t>
+          <t>Lance Stroll</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Haas</t>
+          <t>Aston Martin</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -791,28 +791,28 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>0:01:21.147089</t>
+          <t>0:01:29.462654</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Pierre Gasly</t>
+          <t>Nikita Mazepin</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Alpha Tauri</t>
+          <t>Haas</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -821,28 +821,28 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>0:01:21.238110</t>
+          <t>0:01:29.464090</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Sergio Pérez</t>
+          <t>Yuki Tsunoda</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Red Bull</t>
+          <t>Alpha Tauri</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -851,28 +851,28 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0:01:21.392578</t>
+          <t>0:01:29.507213</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lance Stroll</t>
+          <t>Antonio Giovinazzi</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Aston Martin</t>
+          <t>Alfa-Romeo</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -881,28 +881,28 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0:01:21.507750</t>
+          <t>0:01:29.523189</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>George Russel</t>
+          <t>Pierre Gasly</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Alpha Tauri</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -911,28 +911,28 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0:01:21.580007</t>
+          <t>0:01:29.526840</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kimi Raikkonen</t>
+          <t>Sergio Pérez</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Alfa-Romeo</t>
+          <t>Red Bull</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -941,28 +941,28 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0:01:21.585747</t>
+          <t>0:01:29.544101</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Yuki Tsunoda</t>
+          <t>Kimi Raikkonen</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Alpha Tauri</t>
+          <t>Alfa-Romeo</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0:01:21.685020</t>
+          <t>0:01:29.577895</t>
         </is>
       </c>
     </row>
@@ -1001,28 +1001,28 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0:01:21.782664</t>
+          <t>0:01:30.149072</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Max Verstappen</t>
+          <t>George Russel</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Red Bull</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1031,28 +1031,28 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0:01:21.842005</t>
+          <t>0:01:30.188002</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Antonio Giovinazzi</t>
+          <t>Sebastian Vettel</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Alfa-Romeo</t>
+          <t>Aston Martin</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0:01:21.861092</t>
+          <t>0:01:30.361087</t>
         </is>
       </c>
     </row>

</xml_diff>